<commit_message>
Added NROC and Weekend Allowance + CPIH Selection
</commit_message>
<xml_diff>
--- a/CalculationFile.xlsx
+++ b/CalculationFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/WebDevProjects/pythonpaycalculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9319494-D83B-C541-B476-A5F38C526377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD028155-8BAB-3846-A370-84EBED8AEF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{9F49DC5C-6A96-2841-848A-529403C530C8}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>FY1</t>
-  </si>
-  <si>
-    <t>Number of Hours Worked</t>
   </si>
   <si>
     <t>Unsocial Enhancement per Hour multiplier for base rate</t>
@@ -54,9 +51,6 @@
     <t xml:space="preserve">Source BMA </t>
   </si>
   <si>
-    <t>As the FY1 Table demonstrates it is possible to identify the multipliers which are applied to your base salary when you work either additional or antisocial hours. These are consistent and can be applied across all grades as can be seen in FY2 Table 2 which was calculated using these multiplies dynamically.</t>
-  </si>
-  <si>
     <t>Number of Additional Hours Worked</t>
   </si>
   <si>
@@ -64,6 +58,73 @@
   </si>
   <si>
     <t>Antisocial Hours</t>
+  </si>
+  <si>
+    <t>Number of  Hours Worked</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Weekend Allowance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+For calculation of Weekend Allowance please see BMA link. It is calculated on the principle of a 0 - 0.15 multiplies applied to base salary depending on user selection</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Antisocial and Additional Hours Calculation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+As the FY1 Table demonstrates it is possible to identify the multipliers which are applied to your base salary when you work either additional or antisocial hours. These are consistent and can be applied across all grades as can be seen in FY2 Table 2 which was calculated using these multiplies dynamically.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NROC Calculation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This is based on a 0.08 Multiplier applied to the base salary.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -163,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -183,9 +244,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -193,6 +251,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -511,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6991B2C6-2634-6E4C-B2F6-3EB950B9731A}">
   <dimension ref="B1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,11 +587,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="24">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -542,7 +606,7 @@
     </row>
     <row r="2" spans="2:20" ht="19">
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -578,12 +642,12 @@
         <v>20</v>
       </c>
       <c r="N2" s="4"/>
-      <c r="O2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
+      <c r="O2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
@@ -611,10 +675,10 @@
         <v>1.1849833379616772</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
@@ -643,10 +707,10 @@
         <v>1.2100111080255485</v>
       </c>
       <c r="N4" s="4"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
@@ -675,10 +739,10 @@
         <v>1.2350041655095807</v>
       </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
@@ -707,10 +771,10 @@
         <v>1.2599972229936129</v>
       </c>
       <c r="N6" s="4"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
@@ -739,10 +803,10 @@
         <v>1.2849902804776452</v>
       </c>
       <c r="N7" s="4"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
     </row>
@@ -771,10 +835,10 @@
         <v>1.3099833379616772</v>
       </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
@@ -803,10 +867,10 @@
         <v>1.3350111080255485</v>
       </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
@@ -835,10 +899,10 @@
         <v>1.3600041655095807</v>
       </c>
       <c r="N10" s="4"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
@@ -867,16 +931,16 @@
         <v>1.3849972229936129</v>
       </c>
       <c r="N11" s="4"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
     <row r="12" spans="2:20" ht="21">
       <c r="B12" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -896,7 +960,9 @@
         <v>0.20001388503193551</v>
       </c>
       <c r="N13" s="4"/>
-      <c r="O13" s="10"/>
+      <c r="O13" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
@@ -905,14 +971,14 @@
     </row>
     <row r="14" spans="2:20" ht="16" customHeight="1">
       <c r="B14" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
         <f xml:space="preserve"> C13 / 20</f>
         <v>9.2491668980838604E-3</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="9">
@@ -920,57 +986,57 @@
         <v>2.5001735628991939E-2</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
     </row>
     <row r="15" spans="2:20">
       <c r="B15" s="8"/>
-      <c r="C15" s="12"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="9"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
     </row>
     <row r="16" spans="2:20">
       <c r="B16" s="8"/>
-      <c r="C16" s="12"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
     </row>
     <row r="17" spans="2:20">
       <c r="F17" s="1"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
     </row>
     <row r="18" spans="2:20" ht="24">
-      <c r="B18" s="13" t="s">
-        <v>4</v>
+      <c r="B18" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -983,16 +1049,16 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
     <row r="19" spans="2:20" ht="16" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1075,6 +1141,12 @@
         <f>$C$20+($C$20*($F$14*B20))+($C$20*($M$19*$C$14))</f>
         <v>39513.269404332124</v>
       </c>
+      <c r="O20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
     </row>
     <row r="21" spans="2:20">
       <c r="B21">
@@ -1124,6 +1196,10 @@
         <f t="shared" ref="M21:M28" si="9">$C$20+($C$20*($F$14*B21))+($C$20*($M$19*$C$14))</f>
         <v>40346.952278880861</v>
       </c>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
     </row>
     <row r="22" spans="2:20">
       <c r="B22">
@@ -1173,6 +1249,10 @@
         <f t="shared" si="9"/>
         <v>41180.635153429597</v>
       </c>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
     </row>
     <row r="23" spans="2:20">
       <c r="B23">
@@ -1222,6 +1302,10 @@
         <f t="shared" si="9"/>
         <v>42014.318027978334</v>
       </c>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
     </row>
     <row r="24" spans="2:20">
       <c r="B24">
@@ -1472,11 +1556,11 @@
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="2:20" ht="24">
-      <c r="B30" s="13" t="s">
-        <v>8</v>
+      <c r="B30" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -1491,7 +1575,7 @@
     </row>
     <row r="31" spans="2:20" ht="19">
       <c r="B31" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1725,11 +1809,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="O13:R13"/>
+  <mergeCells count="10">
     <mergeCell ref="C18:M18"/>
     <mergeCell ref="C30:M30"/>
     <mergeCell ref="C1:M1"/>
+    <mergeCell ref="O13:R18"/>
+    <mergeCell ref="O20:R23"/>
     <mergeCell ref="D14:E16"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="F14:F16"/>

</xml_diff>